<commit_message>
added color restore in master fixed in stock check button fixed export data columns fixed E issue in ID
</commit_message>
<xml_diff>
--- a/Supply_2.0_Exported_Data.xlsx
+++ b/Supply_2.0_Exported_Data.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marvin Ma\Desktop\projects\SupplyExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\projects\SupplyExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A843522-C3B2-4116-A0EA-F7667FF53416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AED9F3B-E7EF-4417-B306-971CF8BD9981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="33749" windowHeight="18471" xr2:uid="{3947171F-D80F-4E90-A922-690D6772A658}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{BDEC7189-6851-4962-8047-7D03075D452C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
   <si>
     <t>Clark</t>
   </si>
@@ -143,6 +143,9 @@
     <t>747A9E83</t>
   </si>
   <si>
+    <t>17 1/2</t>
+  </si>
+  <si>
     <t>XL</t>
   </si>
   <si>
@@ -192,6 +195,9 @@
   </si>
   <si>
     <t>6436</t>
+  </si>
+  <si>
+    <t>(2XS / 2TP)</t>
   </si>
   <si>
     <t>6426</t>
@@ -211,7 +217,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -294,39 +300,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -378,7 +384,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -489,6 +495,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -497,13 +510,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -568,46 +574,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1CCEFC-BED7-44B6-98AF-4F60F2862AB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFA4980-C59E-4472-BD7D-2DC34D3EDDAA}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -675,8 +661,8 @@
       <c r="Y1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>12</v>
+      <c r="Z1" s="1">
+        <v>7656</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>11</v>
@@ -694,7 +680,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -764,8 +750,8 @@
       <c r="Y2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>21</v>
+      <c r="Z2" s="1">
+        <v>7644</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>11</v>
@@ -783,7 +769,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -853,8 +839,8 @@
       <c r="Y3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Z3" s="3" t="s">
-        <v>28</v>
+      <c r="Z3" s="3">
+        <v>7040</v>
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="3" t="s">
@@ -867,7 +853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -907,20 +893,20 @@
       <c r="M4" s="1">
         <v>7644</v>
       </c>
-      <c r="N4" s="1">
-        <v>17.5</v>
+      <c r="N4" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="1">
-        <v>7.5</v>
+        <v>36</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>18</v>
@@ -934,17 +920,17 @@
       </c>
       <c r="W4" s="2"/>
       <c r="X4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>35</v>
+      <c r="Z4" s="1">
+        <v>7648</v>
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AC4" t="s">
         <v>34</v>
@@ -953,12 +939,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -1009,7 +995,7 @@
         <v>30</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T5" s="2"/>
       <c r="U5" s="1">
@@ -1025,8 +1011,8 @@
       <c r="Y5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Z5" s="3" t="s">
-        <v>28</v>
+      <c r="Z5" s="3">
+        <v>6444</v>
       </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="3" t="s">
@@ -1039,12 +1025,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -1077,13 +1063,13 @@
         <v>6432</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N6" s="4">
         <v>13</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P6" s="4">
         <v>7</v>
@@ -1092,13 +1078,13 @@
         <v>30</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U6" s="4">
         <v>6432</v>
@@ -1113,26 +1099,26 @@
       <c r="Y6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Z6" s="4" t="s">
-        <v>28</v>
+      <c r="Z6" s="4">
+        <v>6436</v>
       </c>
       <c r="AA6" s="2"/>
       <c r="AB6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AC6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AD6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -1171,7 +1157,7 @@
         <v>13</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P7" s="4">
         <v>7</v>
@@ -1180,13 +1166,13 @@
         <v>30</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U7" s="4">
         <v>6432</v>
@@ -1201,26 +1187,26 @@
       <c r="Y7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Z7" s="4" t="s">
-        <v>28</v>
+      <c r="Z7" s="4">
+        <v>6436</v>
       </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AC7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AD7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -1250,16 +1236,16 @@
         <v>95</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="O8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>31</v>
@@ -1268,31 +1254,31 @@
         <v>7</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>11</v>
@@ -1301,18 +1287,18 @@
         <v>18</v>
       </c>
       <c r="AC8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AD8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -1351,7 +1337,7 @@
         <v>13</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P9" s="4">
         <v>7</v>
@@ -1360,13 +1346,13 @@
         <v>30</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U9" s="4">
         <v>6432</v>
@@ -1381,15 +1367,15 @@
       <c r="Y9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Z9" s="4" t="s">
-        <v>28</v>
+      <c r="Z9" s="4">
+        <v>6436</v>
       </c>
       <c r="AA9" s="2"/>
       <c r="AB9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AC9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AD9" t="s">
         <v>27</v>

</xml_diff>